<commit_message>
Actualizacion estilos general - 9-2-22
</commit_message>
<xml_diff>
--- a/Capturas pantalla .git.xlsx
+++ b/Capturas pantalla .git.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>chequeo git sin iniciar</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>otro git status</t>
-  </si>
-  <si>
-    <t>aca es donde no entido porque una vez que me cambio de rama, me desaparece la rama master--dev2</t>
   </si>
   <si>
     <t>agrego los archivos</t>
@@ -984,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K7:K422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="K422" sqref="K422"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K331" sqref="K331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1197,7 @@
     </row>
     <row r="273" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K273" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="278" spans="11:11" x14ac:dyDescent="0.25">
@@ -1220,22 +1217,17 @@
     </row>
     <row r="318" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K318" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="330" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K330" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="331" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K331" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="336" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K336" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="344" spans="11:11" x14ac:dyDescent="0.25">
@@ -1245,42 +1237,42 @@
     </row>
     <row r="354" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K354" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="370" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K370" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="375" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K375" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="393" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K393" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="404" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K404" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="412" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K412" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="418" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K418" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="422" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K422" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>